<commit_message>
summary of latest rounds of m,l,xl,xxl sample pool tests
</commit_message>
<xml_diff>
--- a/other/test-journals/2023-01-07/Summary.xlsx
+++ b/other/test-journals/2023-01-07/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\crypto\code\repos\KeyScanner\other\test-journals\2023-01-07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFE9445-62F0-4274-855B-7415B4911BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245A7002-2ECE-4783-8887-4CE4201E42CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1455" windowWidth="16065" windowHeight="15555" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18705" yWindow="855" windowWidth="16065" windowHeight="15555" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="460x256" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="(L) 460x256 (Round 2)" sheetId="8" r:id="rId4"/>
     <sheet name="(XL) 460x256" sheetId="9" r:id="rId5"/>
     <sheet name="(XL) 460x256 (Round2)" sheetId="10" r:id="rId6"/>
+    <sheet name="(XXL) 460x256 (2)" sheetId="12" r:id="rId7"/>
+    <sheet name="(XXL) 460x256 (Round 2)" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="7">
   <si>
     <t>Minutes</t>
   </si>
@@ -1934,7 +1936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C7BAF5-8435-421C-B13E-0246B4E818A6}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2242,4 +2244,252 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF5AFC3-FD33-4D12-8B16-8C12E747AEB9}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>128</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>11.13</v>
+      </c>
+      <c r="D6">
+        <f>C6-((B6*K5)/60)</f>
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>128</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f>C7-((B7*K5)/60)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>128</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0.13</v>
+      </c>
+      <c r="D8">
+        <f>C8-((B8*K5)/60)</f>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0.36</v>
+      </c>
+      <c r="D9">
+        <f>C9-((B9*K5)/60)</f>
+        <v>0.36</v>
+      </c>
+      <c r="F9">
+        <f>AVERAGE(C6:C9)</f>
+        <v>3.1550000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(C6:C9)</f>
+        <v>3.1550000000000002</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(D6:D9)</f>
+        <v>1.08</v>
+      </c>
+      <c r="F12">
+        <f>AVERAGE(F2:F9)</f>
+        <v>3.1550000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3481BEEA-04CE-47B5-BD0A-BD68A084CC4C}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>128</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0.33</v>
+      </c>
+      <c r="D6">
+        <f>C6-((B6*K5)/60)</f>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>128</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0.11</v>
+      </c>
+      <c r="D7">
+        <f>C7-((B7*K5)/60)</f>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>128</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0.45</v>
+      </c>
+      <c r="D8">
+        <f>C8-((B8*K5)/60)</f>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0.47</v>
+      </c>
+      <c r="D9">
+        <f>C9-((B9*K5)/60)</f>
+        <v>0.47</v>
+      </c>
+      <c r="F9">
+        <f>AVERAGE(C6:C9)</f>
+        <v>0.33999999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(C6:C9)</f>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(D6:D9)</f>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="F12">
+        <f>AVERAGE(F2:F9)</f>
+        <v>0.33999999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>